<commit_message>
update likelihood and fitting
</commit_message>
<xml_diff>
--- a/Estimated_State_MMR_Uptake_0_to_4.xlsx
+++ b/Estimated_State_MMR_Uptake_0_to_4.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="318" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="424" uniqueCount="106">
   <si>
     <t>State</t>
   </si>
@@ -413,7 +413,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="0">
-        <v>0.67503903249141606</v>
+        <v>0.67789221829395441</v>
       </c>
     </row>
     <row r="3">
@@ -427,7 +427,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="0">
-        <v>0.63263812076442005</v>
+        <v>0.63662190843520516</v>
       </c>
     </row>
     <row r="4">
@@ -441,7 +441,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="0">
-        <v>0.65351824631258748</v>
+        <v>0.65763096820159372</v>
       </c>
     </row>
     <row r="5">
@@ -455,7 +455,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="0">
-        <v>0.66444724503707653</v>
+        <v>0.66981387512608215</v>
       </c>
     </row>
     <row r="6">
@@ -469,7 +469,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="0">
-        <v>0.66568025169570033</v>
+        <v>0.66981309319895665</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="0">
-        <v>0.66614811686071451</v>
+        <v>0.66994337523819347</v>
       </c>
     </row>
     <row r="8">
@@ -497,7 +497,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="0">
-        <v>0.72603493157816867</v>
+        <v>0.72233867299461274</v>
       </c>
     </row>
     <row r="9">
@@ -511,7 +511,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="0">
-        <v>0.6633529583318144</v>
+        <v>0.6700321169479786</v>
       </c>
     </row>
     <row r="10">
@@ -525,7 +525,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="0">
-        <v>0.66735643263757116</v>
+        <v>0.6669743959519292</v>
       </c>
     </row>
     <row r="11">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="0">
-        <v>0.69063638271931038</v>
+        <v>0.69619952087491499</v>
       </c>
     </row>
     <row r="12">
@@ -553,7 +553,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="0">
-        <v>0.65625354911137168</v>
+        <v>0.66737853952129467</v>
       </c>
     </row>
     <row r="13">
@@ -567,7 +567,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="0">
-        <v>0.69329899046838173</v>
+        <v>0.69412808752690369</v>
       </c>
     </row>
     <row r="14">
@@ -595,7 +595,7 @@
         <v>17</v>
       </c>
       <c r="D15" s="0">
-        <v>0.7077446870711771</v>
+        <v>0.70181120458206547</v>
       </c>
     </row>
     <row r="16">
@@ -609,7 +609,7 @@
         <v>18</v>
       </c>
       <c r="D16" s="0">
-        <v>0.68581123072618289</v>
+        <v>0.6785643000554713</v>
       </c>
     </row>
     <row r="17">
@@ -623,7 +623,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="0">
-        <v>0.660270084782142</v>
+        <v>0.66355568254990338</v>
       </c>
     </row>
     <row r="18">
@@ -637,7 +637,7 @@
         <v>20</v>
       </c>
       <c r="D18" s="0">
-        <v>0.69528978551927367</v>
+        <v>0.70047026737419282</v>
       </c>
     </row>
     <row r="19">
@@ -651,7 +651,7 @@
         <v>21</v>
       </c>
       <c r="D19" s="0">
-        <v>0.67087900594029626</v>
+        <v>0.68524113843146095</v>
       </c>
     </row>
     <row r="20">
@@ -665,7 +665,7 @@
         <v>22</v>
       </c>
       <c r="D20" s="0">
-        <v>0.67664778655802738</v>
+        <v>0.68291066818134882</v>
       </c>
     </row>
     <row r="21">
@@ -679,7 +679,7 @@
         <v>23</v>
       </c>
       <c r="D21" s="0">
-        <v>0.71190988070539418</v>
+        <v>0.71296602697095435</v>
       </c>
     </row>
     <row r="22">
@@ -693,7 +693,7 @@
         <v>24</v>
       </c>
       <c r="D22" s="0">
-        <v>0.73642950207551294</v>
+        <v>0.73121809200352961</v>
       </c>
     </row>
     <row r="23">
@@ -707,7 +707,7 @@
         <v>25</v>
       </c>
       <c r="D23" s="0">
-        <v>0.73379005830592881</v>
+        <v>0.72692201185717209</v>
       </c>
     </row>
     <row r="24">
@@ -721,7 +721,7 @@
         <v>26</v>
       </c>
       <c r="D24" s="0">
-        <v>0.71451872154010321</v>
+        <v>0.71849866060023149</v>
       </c>
     </row>
     <row r="25">
@@ -735,7 +735,7 @@
         <v>27</v>
       </c>
       <c r="D25" s="0">
-        <v>0.69419885371328249</v>
+        <v>0.69043666416593508</v>
       </c>
     </row>
     <row r="26">
@@ -749,7 +749,7 @@
         <v>28</v>
       </c>
       <c r="D26" s="0">
-        <v>0.67260202470830477</v>
+        <v>0.67749262182566916</v>
       </c>
     </row>
     <row r="27">
@@ -763,7 +763,7 @@
         <v>29</v>
       </c>
       <c r="D27" s="0">
-        <v>0.70458474554646056</v>
+        <v>0.69667395526471732</v>
       </c>
     </row>
     <row r="28">
@@ -777,7 +777,7 @@
         <v>30</v>
       </c>
       <c r="D28" s="0">
-        <v>0.63597143655283195</v>
+        <v>0.64393686709965769</v>
       </c>
     </row>
     <row r="29">
@@ -791,7 +791,7 @@
         <v>31</v>
       </c>
       <c r="D29" s="0">
-        <v>0.71417451472462967</v>
+        <v>0.7098582699261563</v>
       </c>
     </row>
     <row r="30">
@@ -805,7 +805,7 @@
         <v>32</v>
       </c>
       <c r="D30" s="0">
-        <v>0.65513148349129147</v>
+        <v>0.66625236937255883</v>
       </c>
     </row>
     <row r="31">
@@ -819,7 +819,7 @@
         <v>33</v>
       </c>
       <c r="D31" s="0">
-        <v>0.73185602646466585</v>
+        <v>0.73555820308754438</v>
       </c>
     </row>
     <row r="32">
@@ -833,7 +833,7 @@
         <v>34</v>
       </c>
       <c r="D32" s="0">
-        <v>0.66179267620412641</v>
+        <v>0.65147372382932933</v>
       </c>
     </row>
     <row r="33">
@@ -847,7 +847,7 @@
         <v>35</v>
       </c>
       <c r="D33" s="0">
-        <v>0.6730601723678038</v>
+        <v>0.67892409930004327</v>
       </c>
     </row>
     <row r="34">
@@ -861,7 +861,7 @@
         <v>36</v>
       </c>
       <c r="D34" s="0">
-        <v>0.67904187805148053</v>
+        <v>0.67328727911957031</v>
       </c>
     </row>
     <row r="35">
@@ -875,7 +875,7 @@
         <v>37</v>
       </c>
       <c r="D35" s="0">
-        <v>0.71239471738934457</v>
+        <v>0.72185349483294137</v>
       </c>
     </row>
     <row r="36">
@@ -889,7 +889,7 @@
         <v>38</v>
       </c>
       <c r="D36" s="0">
-        <v>0.66920507536267015</v>
+        <v>0.6720543500222248</v>
       </c>
     </row>
     <row r="37">
@@ -903,7 +903,7 @@
         <v>39</v>
       </c>
       <c r="D37" s="0">
-        <v>0.68852076263240358</v>
+        <v>0.69746488696925146</v>
       </c>
     </row>
     <row r="38">
@@ -917,7 +917,7 @@
         <v>40</v>
       </c>
       <c r="D38" s="0">
-        <v>0.69460654943031608</v>
+        <v>0.68862360939683165</v>
       </c>
     </row>
     <row r="39">
@@ -931,7 +931,7 @@
         <v>41</v>
       </c>
       <c r="D39" s="0">
-        <v>0.68830499128568201</v>
+        <v>0.6951508413994113</v>
       </c>
     </row>
     <row r="40">
@@ -945,7 +945,7 @@
         <v>42</v>
       </c>
       <c r="D40" s="0">
-        <v>0.66523322928138406</v>
+        <v>0.67936949300451122</v>
       </c>
     </row>
     <row r="41">
@@ -973,7 +973,7 @@
         <v>45</v>
       </c>
       <c r="D42" s="0">
-        <v>0.67424911500950691</v>
+        <v>0.67749962620459414</v>
       </c>
     </row>
     <row r="43">
@@ -987,7 +987,7 @@
         <v>46</v>
       </c>
       <c r="D43" s="0">
-        <v>0.68956079731911868</v>
+        <v>0.69890255760248643</v>
       </c>
     </row>
     <row r="44">
@@ -1001,7 +1001,7 @@
         <v>47</v>
       </c>
       <c r="D44" s="0">
-        <v>0.70332804453891107</v>
+        <v>0.69763079319839627</v>
       </c>
     </row>
     <row r="45">
@@ -1015,7 +1015,7 @@
         <v>48</v>
       </c>
       <c r="D45" s="0">
-        <v>0.70741910771540362</v>
+        <v>0.71067323586547015</v>
       </c>
     </row>
     <row r="46">
@@ -1029,7 +1029,7 @@
         <v>49</v>
       </c>
       <c r="D46" s="0">
-        <v>0.69492897992555458</v>
+        <v>0.6990675430858273</v>
       </c>
     </row>
     <row r="47">
@@ -1043,7 +1043,7 @@
         <v>50</v>
       </c>
       <c r="D47" s="0">
-        <v>0.73443570933245739</v>
+        <v>0.73104171685098007</v>
       </c>
     </row>
     <row r="48">
@@ -1057,7 +1057,7 @@
         <v>51</v>
       </c>
       <c r="D48" s="0">
-        <v>0.67720438856371101</v>
+        <v>0.68884856819917761</v>
       </c>
     </row>
     <row r="49">
@@ -1071,7 +1071,7 @@
         <v>53</v>
       </c>
       <c r="D49" s="0">
-        <v>0.69548795119663021</v>
+        <v>0.70203227943135027</v>
       </c>
     </row>
     <row r="50">
@@ -1085,7 +1085,7 @@
         <v>54</v>
       </c>
       <c r="D50" s="0">
-        <v>0.65626572236657532</v>
+        <v>0.65276166386902434</v>
       </c>
     </row>
     <row r="51">
@@ -1099,7 +1099,7 @@
         <v>55</v>
       </c>
       <c r="D51" s="0">
-        <v>0.70797721337038055</v>
+        <v>0.70714155816654589</v>
       </c>
     </row>
     <row r="52">
@@ -1113,7 +1113,7 @@
         <v>56</v>
       </c>
       <c r="D52" s="0">
-        <v>0.67733865248226943</v>
+        <v>0.69098971631205675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>